<commit_message>
MP1: Migrate most instruments to inf-0 from inf-12
</commit_message>
<xml_diff>
--- a/Analysis/volume-db.xlsx
+++ b/Analysis/volume-db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\app\MGen\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F62C12B-A8FB-4166-AE3B-298A02862020}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCAFA6F-0820-4130-935B-97F9CA36B6DF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{FF9B3C90-53D0-4800-BC43-3A71C311DF65}"/>
   </bookViews>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="20">
   <si>
     <t>Piano</t>
   </si>
@@ -1944,6 +1944,570 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>db</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> to amplitude</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Scales!$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Amplitude</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Scales!$D$10:$P$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Scales!$D$11:$P$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56234132519034907</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.31622776601683794</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17782794100389224</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.6234132519034884E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.1622776601683784E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7782794100389226E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.6234132519034866E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.1622776601683764E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.7782794100389223E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D63A-4C1D-9131-022776E8DAE3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="329026464"/>
+        <c:axId val="519708784"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Scales!$C$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>db</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Scales!$D$10:$P$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="13"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>-5</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>-10</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>-15</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>-20</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>-25</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>-30</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>-35</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>-40</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>-45</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>-50</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>-55</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>-60</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Scales!$D$10:$P$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="13"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>-5</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>-10</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>-15</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>-20</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>-25</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>-30</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>-35</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>-40</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>-45</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>-50</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>-55</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>-60</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-D63A-4C1D-9131-022776E8DAE3}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="329026464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="519708784"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="519708784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="329026464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2024,6 +2588,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3056,20 +3660,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>117157</xdr:colOff>
+      <xdr:colOff>18097</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3096,16 +4216,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>501966</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>103822</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>545781</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>160972</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>169545</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>40005</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3125,6 +4245,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>98107</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>39052</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>402907</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>67627</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67C976C0-9078-4CD2-9A8F-320F3003BB17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3786,7 +4942,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4261,100 +5417,103 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>19</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>0</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>-5</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>-10</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>-15</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>-20</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>-25</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>-30</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>-35</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>-40</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>-45</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>-50</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>-55</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>-60</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C11">
-        <f>POWER(10, C10/20)</f>
-        <v>1</v>
+      <c r="C11" t="s">
+        <v>18</v>
       </c>
       <c r="D11">
         <f>POWER(10, D10/20)</f>
-        <v>0.56234132519034907</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <f>POWER(10, E10/20)</f>
-        <v>0.31622776601683794</v>
+        <v>0.56234132519034907</v>
       </c>
       <c r="F11">
         <f>POWER(10, F10/20)</f>
-        <v>0.17782794100389224</v>
+        <v>0.31622776601683794</v>
       </c>
       <c r="G11">
         <f>POWER(10, G10/20)</f>
-        <v>0.1</v>
+        <v>0.17782794100389224</v>
       </c>
       <c r="H11">
         <f>POWER(10, H10/20)</f>
-        <v>5.6234132519034884E-2</v>
+        <v>0.1</v>
       </c>
       <c r="I11">
         <f>POWER(10, I10/20)</f>
-        <v>3.1622776601683784E-2</v>
+        <v>5.6234132519034884E-2</v>
       </c>
       <c r="J11">
         <f>POWER(10, J10/20)</f>
-        <v>1.7782794100389226E-2</v>
+        <v>3.1622776601683784E-2</v>
       </c>
       <c r="K11">
         <f>POWER(10, K10/20)</f>
-        <v>0.01</v>
+        <v>1.7782794100389226E-2</v>
       </c>
       <c r="L11">
         <f>POWER(10, L10/20)</f>
-        <v>5.6234132519034866E-3</v>
+        <v>0.01</v>
       </c>
       <c r="M11">
         <f>POWER(10, M10/20)</f>
-        <v>3.1622776601683764E-3</v>
+        <v>5.6234132519034866E-3</v>
       </c>
       <c r="N11">
         <f>POWER(10, N10/20)</f>
-        <v>1.7782794100389223E-3</v>
+        <v>3.1622776601683764E-3</v>
       </c>
       <c r="O11">
         <f>POWER(10, O10/20)</f>
+        <v>1.7782794100389223E-3</v>
+      </c>
+      <c r="P11">
+        <f>POWER(10, P10/20)</f>
         <v>1E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MP1: Better dB processing
</commit_message>
<xml_diff>
--- a/Analysis/volume-db.xlsx
+++ b/Analysis/volume-db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\app\MGen\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCAFA6F-0820-4130-935B-97F9CA36B6DF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5205E08E-4727-41AB-AEA0-87812F08DB39}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{FF9B3C90-53D0-4800-BC43-3A71C311DF65}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF9B3C90-53D0-4800-BC43-3A71C311DF65}"/>
   </bookViews>
   <sheets>
     <sheet name="Instr" sheetId="1" r:id="rId1"/>
@@ -389,10 +389,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Scales!$C$5:$P$5</c:f>
+              <c:f>Scales!$C$5:$Q$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>127</c:v>
                 </c:pt>
@@ -432,7 +432,7 @@
                 <c:pt idx="12">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -440,10 +440,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scales!$C$6:$P$6</c:f>
+              <c:f>Scales!$C$6:$Q$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>3.9810717055349727</c:v>
                 </c:pt>
@@ -483,7 +483,7 @@
                 <c:pt idx="12">
                   <c:v>1.9952623149688781E-3</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -524,10 +524,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Scales!$C$5:$P$5</c:f>
+              <c:f>Scales!$C$5:$Q$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>127</c:v>
                 </c:pt>
@@ -567,7 +567,7 @@
                 <c:pt idx="12">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -575,10 +575,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scales!$C$7:$P$7</c:f>
+              <c:f>Scales!$C$7:$Q$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -618,7 +618,7 @@
                 <c:pt idx="12">
                   <c:v>5.0118723362727209E-4</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -659,10 +659,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Scales!$C$5:$P$5</c:f>
+              <c:f>Scales!$C$5:$Q$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>127</c:v>
                 </c:pt>
@@ -702,7 +702,7 @@
                 <c:pt idx="12">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -710,10 +710,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scales!$C$8:$P$8</c:f>
+              <c:f>Scales!$C$8:$Q$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -753,7 +753,7 @@
                 <c:pt idx="12">
                   <c:v>7.9432823472428096E-2</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -817,13 +817,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Scales!$C$5:$P$5</c15:sqref>
+                          <c15:sqref>Scales!$C$5:$Q$5</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="14"/>
+                      <c:ptCount val="15"/>
                       <c:pt idx="0">
                         <c:v>127</c:v>
                       </c:pt>
@@ -863,7 +863,7 @@
                       <c:pt idx="12">
                         <c:v>10</c:v>
                       </c:pt>
-                      <c:pt idx="13">
+                      <c:pt idx="14">
                         <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
@@ -874,13 +874,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Scales!$C$5:$P$5</c15:sqref>
+                          <c15:sqref>Scales!$C$5:$Q$5</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="14"/>
+                      <c:ptCount val="15"/>
                       <c:pt idx="0">
                         <c:v>127</c:v>
                       </c:pt>
@@ -920,7 +920,7 @@
                       <c:pt idx="12">
                         <c:v>10</c:v>
                       </c:pt>
-                      <c:pt idx="13">
+                      <c:pt idx="14">
                         <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
@@ -1230,10 +1230,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Scales!$C$1:$O$1</c:f>
+              <c:f>Scales!$C$1:$P$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>127</c:v>
                 </c:pt>
@@ -1272,16 +1272,19 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scales!$C$2:$O$2</c:f>
+              <c:f>Scales!$C$2:$P$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>12</c:v>
                 </c:pt>
@@ -1320,6 +1323,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>-54</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-113.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1359,10 +1365,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Scales!$C$1:$O$1</c:f>
+              <c:f>Scales!$C$1:$P$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>127</c:v>
                 </c:pt>
@@ -1401,16 +1407,19 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scales!$C$3:$O$3</c:f>
+              <c:f>Scales!$C$3:$P$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1449,6 +1458,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>-66</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-125.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1488,10 +1500,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Scales!$C$1:$O$1</c:f>
+              <c:f>Scales!$C$1:$P$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>127</c:v>
                 </c:pt>
@@ -1530,16 +1542,19 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scales!$C$4:$O$4</c:f>
+              <c:f>Scales!$C$4:$P$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1578,6 +1593,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>-22</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1586,6 +1604,311 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-9DF1-4065-83AD-87110DF86D1C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Scales!$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3750</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Scales!$C$1:$P$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Scales!$C$12:$P$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.1522273836578618</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.770404685813078</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-6.2689478292711485</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-9.0290199339773665</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-12.112109213019556</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-15.604354452176949</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-19.631798537577406</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-24.389647552571503</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-30.204526409772502</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-37.687818346172769</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-48.209371274345884</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-66.127067681188564</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-125.02812238545616</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-9DF1-4065-83AD-87110DF86D1C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Scales!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1250</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Scales!$C$13:$P$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.71740912788595401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.2568015619376927</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.0896492764237165</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-3.009673311325789</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-4.0373697376731856</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-5.2014514840589836</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-6.5439328458591355</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-8.1298825175238338</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-10.068175469924167</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-12.562606115390922</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-16.06979042478196</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-22.042355893729521</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-41.676040795152055</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-9DF1-4065-83AD-87110DF86D1C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Scales!$B$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3750</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Scales!$C$14:$P$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.8477726163421373</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.2295953141869216</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.7310521707288515</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9709800660226335</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.11210921301955601</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-3.6043544521769491</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-7.6317985375774064</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-12.389647552571503</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-18.204526409772502</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-25.687818346172769</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-36.209371274345884</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-54.127067681188564</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-113.02812238545616</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-9DF1-4065-83AD-87110DF86D1C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1640,13 +1963,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Scales!$C$1:$O$1</c15:sqref>
+                          <c15:sqref>Scales!$C$1:$P$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="13"/>
+                      <c:ptCount val="14"/>
                       <c:pt idx="0">
                         <c:v>127</c:v>
                       </c:pt>
@@ -1685,6 +2008,9 @@
                       </c:pt>
                       <c:pt idx="12">
                         <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>1</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2052,10 +2378,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Scales!$D$10:$P$10</c:f>
+              <c:f>Scales!$D$10:$Q$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2092,7 +2418,7 @@
                 <c:pt idx="11">
                   <c:v>-55</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>-60</c:v>
                 </c:pt>
               </c:numCache>
@@ -2100,10 +2426,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scales!$D$11:$P$11</c:f>
+              <c:f>Scales!$D$11:$Q$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2140,7 +2466,7 @@
                 <c:pt idx="11">
                   <c:v>1.7782794100389223E-3</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>1E-3</c:v>
                 </c:pt>
               </c:numCache>
@@ -2204,13 +2530,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Scales!$D$10:$P$10</c15:sqref>
+                          <c15:sqref>Scales!$D$10:$Q$10</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="13"/>
+                      <c:ptCount val="14"/>
                       <c:pt idx="0">
                         <c:v>0</c:v>
                       </c:pt>
@@ -2247,7 +2573,7 @@
                       <c:pt idx="11">
                         <c:v>-55</c:v>
                       </c:pt>
-                      <c:pt idx="12">
+                      <c:pt idx="13">
                         <c:v>-60</c:v>
                       </c:pt>
                     </c:numCache>
@@ -2258,13 +2584,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Scales!$D$10:$P$10</c15:sqref>
+                          <c15:sqref>Scales!$D$10:$Q$10</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="13"/>
+                      <c:ptCount val="14"/>
                       <c:pt idx="0">
                         <c:v>0</c:v>
                       </c:pt>
@@ -2301,7 +2627,7 @@
                       <c:pt idx="11">
                         <c:v>-55</c:v>
                       </c:pt>
-                      <c:pt idx="12">
+                      <c:pt idx="13">
                         <c:v>-60</c:v>
                       </c:pt>
                     </c:numCache>
@@ -4180,15 +4506,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>18097</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4216,16 +4542,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>545781</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>160972</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>35241</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>139065</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:colOff>300990</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>40005</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4252,15 +4578,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>98107</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>39052</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
+      <xdr:col>37</xdr:col>
       <xdr:colOff>402907</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>67627</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4589,13 +4915,13 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -4645,7 +4971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -4695,7 +5021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -4745,7 +5071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -4760,7 +5086,7 @@
       </c>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -4810,7 +5136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -4822,7 +5148,7 @@
       </c>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -4836,7 +5162,7 @@
         <v>-15.5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -4856,7 +5182,7 @@
         <v>-36</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -4867,7 +5193,7 @@
         <v>-6.2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -4878,7 +5204,7 @@
         <v>-12.2</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -4889,7 +5215,7 @@
         <v>-12.2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -4900,33 +5226,33 @@
         <v>-6.2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I13">
-        <f>I1*127/80</f>
+        <f t="shared" ref="I13:O13" si="0">I1*127/80</f>
         <v>111.125</v>
       </c>
       <c r="J13">
-        <f>J1*127/80</f>
+        <f t="shared" si="0"/>
         <v>95.25</v>
       </c>
       <c r="K13">
-        <f>K1*127/80</f>
+        <f t="shared" si="0"/>
         <v>79.375</v>
       </c>
       <c r="L13">
-        <f>L1*127/80</f>
+        <f t="shared" si="0"/>
         <v>63.5</v>
       </c>
       <c r="M13">
-        <f>M1*127/80</f>
+        <f t="shared" si="0"/>
         <v>47.625</v>
       </c>
       <c r="N13">
-        <f>N1*127/80</f>
+        <f t="shared" si="0"/>
         <v>31.75</v>
       </c>
       <c r="O13">
-        <f>O1*127/80</f>
+        <f t="shared" si="0"/>
         <v>15.875</v>
       </c>
     </row>
@@ -4939,15 +5265,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FC5F2D-347C-4DC5-A03A-93E6273B89F3}">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -4994,10 +5320,13 @@
         <v>10</v>
       </c>
       <c r="P1" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -5043,11 +5372,14 @@
       <c r="O2" s="1">
         <v>-54</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="1">
+        <v>-113.8</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -5093,11 +5425,14 @@
       <c r="O3">
         <v>-66</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P3">
+        <v>-125.8</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -5143,11 +5478,14 @@
       <c r="O4">
         <v>-22</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4">
+        <v>-42</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -5193,11 +5531,12 @@
       <c r="O5" s="3">
         <v>10</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -5205,218 +5544,218 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <f>POWER(10, C2/20)</f>
+        <f t="shared" ref="C6:O6" si="0">POWER(10, C2/20)</f>
         <v>3.9810717055349727</v>
       </c>
       <c r="D6">
-        <f>POWER(10, D2/20)</f>
+        <f t="shared" si="0"/>
         <v>3.1260793671239555</v>
       </c>
       <c r="E6">
-        <f>POWER(10, E2/20)</f>
+        <f t="shared" si="0"/>
         <v>2.6001595631652723</v>
       </c>
       <c r="F6">
-        <f>POWER(10, F2/20)</f>
+        <f t="shared" si="0"/>
         <v>1.9498445997580454</v>
       </c>
       <c r="G6">
-        <f>POWER(10, G2/20)</f>
+        <f t="shared" si="0"/>
         <v>1.4288939585111029</v>
       </c>
       <c r="H6">
-        <f>POWER(10, H2/20)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I6">
-        <f>POWER(10, I2/20)</f>
+        <f t="shared" si="0"/>
         <v>0.66834391756861455</v>
       </c>
       <c r="J6">
-        <f>POWER(10, J2/20)</f>
+        <f t="shared" si="0"/>
         <v>0.42169650342858223</v>
       </c>
       <c r="K6">
-        <f>POWER(10, K2/20)</f>
+        <f t="shared" si="0"/>
         <v>0.24547089156850299</v>
       </c>
       <c r="L6">
-        <f>POWER(10, L2/20)</f>
+        <f t="shared" si="0"/>
         <v>0.12589254117941667</v>
       </c>
       <c r="M6">
-        <f>POWER(10, M2/20)</f>
+        <f t="shared" si="0"/>
         <v>5.3088444423098825E-2</v>
       </c>
       <c r="N6">
-        <f>POWER(10, N2/20)</f>
+        <f t="shared" si="0"/>
         <v>1.5848931924611124E-2</v>
       </c>
       <c r="O6">
-        <f>POWER(10, O2/20)</f>
+        <f t="shared" si="0"/>
         <v>1.9952623149688781E-3</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7">
-        <f>POWER(10, C3/20)</f>
+        <f t="shared" ref="C7:O7" si="1">POWER(10, C3/20)</f>
         <v>1</v>
       </c>
       <c r="D7">
-        <f>POWER(10, D3/20)</f>
+        <f t="shared" si="1"/>
         <v>0.77624711662869172</v>
       </c>
       <c r="E7">
-        <f>POWER(10, E3/20)</f>
+        <f t="shared" si="1"/>
         <v>0.64565422903465541</v>
       </c>
       <c r="F7">
-        <f>POWER(10, F3/20)</f>
+        <f t="shared" si="1"/>
         <v>0.48977881936844614</v>
       </c>
       <c r="G7">
-        <f>POWER(10, G3/20)</f>
+        <f t="shared" si="1"/>
         <v>0.35481338923357542</v>
       </c>
       <c r="H7">
-        <f>POWER(10, H3/20)</f>
+        <f t="shared" si="1"/>
         <v>0.25118864315095801</v>
       </c>
       <c r="I7">
-        <f>POWER(10, I3/20)</f>
+        <f t="shared" si="1"/>
         <v>0.167880401812256</v>
       </c>
       <c r="J7">
-        <f>POWER(10, J3/20)</f>
+        <f t="shared" si="1"/>
         <v>0.10592537251772888</v>
       </c>
       <c r="K7">
-        <f>POWER(10, K3/20)</f>
+        <f t="shared" si="1"/>
         <v>6.1659500186148221E-2</v>
       </c>
       <c r="L7">
-        <f>POWER(10, L3/20)</f>
+        <f t="shared" si="1"/>
         <v>3.1622776601683784E-2</v>
       </c>
       <c r="M7">
-        <f>POWER(10, M3/20)</f>
+        <f t="shared" si="1"/>
         <v>1.333521432163323E-2</v>
       </c>
       <c r="N7">
-        <f>POWER(10, N3/20)</f>
+        <f t="shared" si="1"/>
         <v>3.9810717055349717E-3</v>
       </c>
       <c r="O7">
-        <f>POWER(10, O3/20)</f>
+        <f t="shared" si="1"/>
         <v>5.0118723362727209E-4</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8">
-        <f>POWER(10, C4/20)</f>
+        <f t="shared" ref="C8:O8" si="2">POWER(10, C4/20)</f>
         <v>1</v>
       </c>
       <c r="D8">
-        <f>POWER(10, D4/20)</f>
+        <f t="shared" si="2"/>
         <v>0.92257142715476315</v>
       </c>
       <c r="E8">
-        <f>POWER(10, E4/20)</f>
+        <f t="shared" si="2"/>
         <v>0.87096358995608059</v>
       </c>
       <c r="F8">
-        <f>POWER(10, F4/20)</f>
+        <f t="shared" si="2"/>
         <v>0.79432823472428149</v>
       </c>
       <c r="G8">
-        <f>POWER(10, G4/20)</f>
+        <f t="shared" si="2"/>
         <v>0.70794578438413791</v>
       </c>
       <c r="H8">
-        <f>POWER(10, H4/20)</f>
+        <f t="shared" si="2"/>
         <v>0.63095734448019325</v>
       </c>
       <c r="I8">
-        <f>POWER(10, I4/20)</f>
+        <f t="shared" si="2"/>
         <v>0.55590425727040349</v>
       </c>
       <c r="J8">
-        <f>POWER(10, J4/20)</f>
+        <f t="shared" si="2"/>
         <v>0.47315125896148047</v>
       </c>
       <c r="K8">
-        <f>POWER(10, K4/20)</f>
+        <f t="shared" si="2"/>
         <v>0.3981071705534972</v>
       </c>
       <c r="L8">
-        <f>POWER(10, L4/20)</f>
+        <f t="shared" si="2"/>
         <v>0.31622776601683794</v>
       </c>
       <c r="M8">
-        <f>POWER(10, M4/20)</f>
+        <f t="shared" si="2"/>
         <v>0.23713737056616549</v>
       </c>
       <c r="N8">
-        <f>POWER(10, N4/20)</f>
+        <f t="shared" si="2"/>
         <v>0.15848931924611132</v>
       </c>
       <c r="O8">
-        <f>POWER(10, O4/20)</f>
+        <f t="shared" si="2"/>
         <v>7.9432823472428096E-2</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="I9">
-        <f>I1*127/80</f>
+        <f t="shared" ref="I9:O9" si="3">I1*127/80</f>
         <v>111.125</v>
       </c>
       <c r="J9">
-        <f>J1*127/80</f>
+        <f t="shared" si="3"/>
         <v>95.25</v>
       </c>
       <c r="K9">
-        <f>K1*127/80</f>
+        <f t="shared" si="3"/>
         <v>79.375</v>
       </c>
       <c r="L9">
-        <f>L1*127/80</f>
+        <f t="shared" si="3"/>
         <v>63.5</v>
       </c>
       <c r="M9">
-        <f>M1*127/80</f>
+        <f t="shared" si="3"/>
         <v>47.625</v>
       </c>
       <c r="N9">
-        <f>N1*127/80</f>
+        <f t="shared" si="3"/>
         <v>31.75</v>
       </c>
       <c r="O9">
-        <f>O1*127/80</f>
+        <f t="shared" si="3"/>
         <v>15.875</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>19</v>
       </c>
@@ -5456,65 +5795,267 @@
       <c r="O10">
         <v>-55</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>-60</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11">
-        <f>POWER(10, D10/20)</f>
+        <f t="shared" ref="D11:O11" si="4">POWER(10, D10/20)</f>
         <v>1</v>
       </c>
       <c r="E11">
-        <f>POWER(10, E10/20)</f>
+        <f t="shared" si="4"/>
         <v>0.56234132519034907</v>
       </c>
       <c r="F11">
-        <f>POWER(10, F10/20)</f>
+        <f t="shared" si="4"/>
         <v>0.31622776601683794</v>
       </c>
       <c r="G11">
-        <f>POWER(10, G10/20)</f>
+        <f t="shared" si="4"/>
         <v>0.17782794100389224</v>
       </c>
       <c r="H11">
-        <f>POWER(10, H10/20)</f>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
       <c r="I11">
-        <f>POWER(10, I10/20)</f>
+        <f t="shared" si="4"/>
         <v>5.6234132519034884E-2</v>
       </c>
       <c r="J11">
-        <f>POWER(10, J10/20)</f>
+        <f t="shared" si="4"/>
         <v>3.1622776601683784E-2</v>
       </c>
       <c r="K11">
-        <f>POWER(10, K10/20)</f>
+        <f t="shared" si="4"/>
         <v>1.7782794100389226E-2</v>
       </c>
       <c r="L11">
-        <f>POWER(10, L10/20)</f>
+        <f t="shared" si="4"/>
         <v>0.01</v>
       </c>
       <c r="M11">
-        <f>POWER(10, M10/20)</f>
+        <f t="shared" si="4"/>
         <v>5.6234132519034866E-3</v>
       </c>
       <c r="N11">
-        <f>POWER(10, N10/20)</f>
+        <f t="shared" si="4"/>
         <v>3.1622776601683764E-3</v>
       </c>
       <c r="O11">
-        <f>POWER(10, O10/20)</f>
+        <f t="shared" si="4"/>
         <v>1.7782794100389223E-3</v>
       </c>
-      <c r="P11">
-        <f>POWER(10, P10/20)</f>
+      <c r="Q11">
+        <f>POWER(10, Q10/20)</f>
         <v>1E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="B12">
+        <v>3750</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f>(POWER(D$1/127, $A12)-1)*$B12</f>
+        <v>-2.1522273836578618</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="E12:P13" si="5">(POWER(E$1/127, $A12)-1)*$B12</f>
+        <v>-3.770404685813078</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="5"/>
+        <v>-6.2689478292711485</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="5"/>
+        <v>-9.0290199339773665</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="5"/>
+        <v>-12.112109213019556</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="5"/>
+        <v>-15.604354452176949</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="5"/>
+        <v>-19.631798537577406</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="5"/>
+        <v>-24.389647552571503</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="5"/>
+        <v>-30.204526409772502</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="5"/>
+        <v>-37.687818346172769</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="5"/>
+        <v>-48.209371274345884</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="5"/>
+        <v>-66.127067681188564</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="5"/>
+        <v>-125.02812238545616</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="B13">
+        <f>B12/3</f>
+        <v>1250</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13" si="6">(POWER(D$1/127, $A13)-1)*$B13</f>
+        <v>-0.71740912788595401</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="5"/>
+        <v>-1.2568015619376927</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="5"/>
+        <v>-2.0896492764237165</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="5"/>
+        <v>-3.009673311325789</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="5"/>
+        <v>-4.0373697376731856</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="5"/>
+        <v>-5.2014514840589836</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="5"/>
+        <v>-6.5439328458591355</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="5"/>
+        <v>-8.1298825175238338</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="5"/>
+        <v>-10.068175469924167</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="5"/>
+        <v>-12.562606115390922</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="5"/>
+        <v>-16.06979042478196</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="5"/>
+        <v>-22.042355893729521</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="5"/>
+        <v>-41.676040795152055</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="B14">
+        <v>3750</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <f>(POWER(D$1/127, $A14)-1)*$B14+12</f>
+        <v>9.8477726163421373</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ref="E14:P14" si="7">(POWER(E$1/127, $A14)-1)*$B14+12</f>
+        <v>8.2295953141869216</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="7"/>
+        <v>5.7310521707288515</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="7"/>
+        <v>2.9709800660226335</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="7"/>
+        <v>-0.11210921301955601</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="7"/>
+        <v>-3.6043544521769491</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="7"/>
+        <v>-7.6317985375774064</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="7"/>
+        <v>-12.389647552571503</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="7"/>
+        <v>-18.204526409772502</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="7"/>
+        <v>-25.687818346172769</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="7"/>
+        <v>-36.209371274345884</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="7"/>
+        <v>-54.127067681188564</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="7"/>
+        <v>-113.02812238545616</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>1/A14</f>
+        <v>142.85714285714286</v>
+      </c>
+    </row>
+    <row r="20" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P20">
+        <f>(POWER(111.75/127, 0.007) - 1) *1250*2</f>
+        <v>-2.237647915296348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MP1: Implement LASS strings
</commit_message>
<xml_diff>
--- a/Analysis/volume-db.xlsx
+++ b/Analysis/volume-db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\app\MGen\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5205E08E-4727-41AB-AEA0-87812F08DB39}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01CD88C-9774-487E-B759-5F39EAFD8BAA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF9B3C90-53D0-4800-BC43-3A71C311DF65}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{FF9B3C90-53D0-4800-BC43-3A71C311DF65}"/>
   </bookViews>
   <sheets>
     <sheet name="Instr" sheetId="1" r:id="rId1"/>
@@ -4543,15 +4543,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>35241</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>139065</xdr:rowOff>
+      <xdr:colOff>16191</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>24765</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>300990</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4915,7 +4915,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -5267,8 +5267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FC5F2D-347C-4DC5-A03A-93E6273B89F3}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>